<commit_message>
Add Forgot Password and Reset Password
</commit_message>
<xml_diff>
--- a/data/list-users.xlsx
+++ b/data/list-users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinhc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IKBO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF530B73-F01E-405B-ADFA-BB52C0962206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA2FB57-9054-45DC-8DC3-46B13284EC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="3420" windowWidth="21675" windowHeight="11340" xr2:uid="{EABF7CD3-D2C2-42F1-A339-1F04FDBFDC53}"/>
+    <workbookView xWindow="1410" yWindow="3105" windowWidth="28800" windowHeight="15345" xr2:uid="{EABF7CD3-D2C2-42F1-A339-1F04FDBFDC53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>avatar.png</t>
   </si>
@@ -42,34 +42,22 @@
     <t>INACTIVE</t>
   </si>
   <si>
-    <t>1@example.com</t>
-  </si>
-  <si>
-    <t>2@example.com</t>
-  </si>
-  <si>
-    <t>3@example.com</t>
-  </si>
-  <si>
-    <t>4@example.com</t>
-  </si>
-  <si>
-    <t>5@example.com</t>
-  </si>
-  <si>
-    <t>6@example.com</t>
-  </si>
-  <si>
-    <t>7@example.com</t>
-  </si>
-  <si>
-    <t>8@example.com</t>
-  </si>
-  <si>
-    <t>9@example.com</t>
-  </si>
-  <si>
-    <t>0@example.com</t>
+    <t>xuancanhit99@gmail.com</t>
+  </si>
+  <si>
+    <t>Lê Đình Cường</t>
+  </si>
+  <si>
+    <t>Vũ Xuân Cảnh</t>
+  </si>
+  <si>
+    <t>Phương Tiến Đông</t>
+  </si>
+  <si>
+    <t>dinhcuong1.firewin99@gmail.com</t>
+  </si>
+  <si>
+    <t>dongpt4101@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -80,7 +68,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -88,13 +76,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -438,26 +426,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C29C03-B844-4865-8DCA-B8A0E3A037DE}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.875" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1">
         <v>123456789</v>
@@ -469,9 +457,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -486,12 +474,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>123456789</v>
@@ -500,125 +488,6 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>123456789</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>123456789</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>123456789</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>123456789</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>123456789</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>123456789</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>123456789</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -626,15 +495,8 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{EA40E2D9-E472-4883-B57B-ABDAFBD06B2C}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{3A0B1548-FC46-4697-86EC-1E5AB1A7725B}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{B70BF70D-FFF2-430E-B898-4BD47F3E84FD}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{2CDC997A-36E8-4B06-BD72-147B2F30A774}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{F9662DA8-5E41-4C4D-924F-E5DD53A63D2C}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{5D87744A-EC95-4F0E-94C3-74BA8F928FFE}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{752E352E-5E0D-42E3-A8B1-89E85944E15A}"/>
-    <hyperlink ref="B8" r:id="rId8" xr:uid="{A463C310-1B8A-49C4-8C0A-B855A8F03D2C}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{72CA6FE1-C269-4E71-89D5-14BED5CBF539}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{4C1F002E-8B3A-428D-8173-70478B139B64}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{514DFFFF-CDCC-B64F-8189-E10178B28D55}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{1234AA86-C099-374F-8FE3-C6DBB3EBD414}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[HOT CHANGE] Fix bug
</commit_message>
<xml_diff>
--- a/data/list-users.xlsx
+++ b/data/list-users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IKBO\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\newXampp\htdocs\mireavn\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA2FB57-9054-45DC-8DC3-46B13284EC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4688EE7A-072E-41B6-B062-EBD67E059B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="3105" windowWidth="28800" windowHeight="15345" xr2:uid="{EABF7CD3-D2C2-42F1-A339-1F04FDBFDC53}"/>
+    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{EABF7CD3-D2C2-42F1-A339-1F04FDBFDC53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>avatar.png</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>dongpt4101@gmail.com</t>
+  </si>
+  <si>
+    <t>Mirea123456789</t>
+  </si>
+  <si>
+    <t>Mirea123456790</t>
+  </si>
+  <si>
+    <t>Mirea123456791</t>
   </si>
 </sst>
 </file>
@@ -68,7 +77,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -76,13 +85,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -429,26 +438,26 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.875" customWidth="1"/>
-    <col min="2" max="2" width="32.875" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1">
-        <v>123456789</v>
+      <c r="C1" t="s">
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -457,15 +466,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>123456789</v>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -474,15 +483,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>123456789</v>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>

</xml_diff>